<commit_message>
zve() function: Child allowance is now transferred among couples if possible.
Former-commit-id: afd4b8e4938b4cde9ca9f510365c36eed1fca766
Former-commit-id: ca0d934174dd23ba5fe552cf1cb9f5a3fdfc7194
</commit_message>
<xml_diff>
--- a/pre-waf/tests/test_data/test_dfs_ssc.xlsx
+++ b/pre-waf/tests/test_data/test_dfs_ssc.xlsx
@@ -106,10 +106,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,7 +418,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,23 +517,22 @@
       </c>
       <c r="L2" s="2">
         <f>R2+S2+T2+U2</f>
-        <v>10.799999999999999</v>
+        <v>0</v>
       </c>
       <c r="Q2">
         <f>0.7547*450+(((850/(850-450))-(450/(850-450)*0.7547))*(C2-450))</f>
         <v>148.22062500000001</v>
       </c>
-      <c r="R2">
-        <f>0.036*C2</f>
-        <v>10.799999999999999</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2">
+      <c r="R2" s="3">
+        <v>0</v>
+      </c>
+      <c r="S2" s="3">
+        <v>0</v>
+      </c>
+      <c r="T2" s="3">
+        <v>0</v>
+      </c>
+      <c r="U2" s="3">
         <v>0</v>
       </c>
     </row>
@@ -579,19 +579,19 @@
         <f t="shared" ref="Q3:Q7" si="2">0.7547*450+(((850/(850-450))-(450/(850-450)*0.7547))*(C3-450))</f>
         <v>531.00937499999998</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="3">
         <f>0.093 * 2 *$Q3 - (0.093 *$C3)</f>
         <v>42.967743749999997</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="3">
         <f>0.01275*2*$Q3-(0.01275*$C3)+(0.0025*(G3=FALSE)*(E3&gt;=23)*Q3)</f>
         <v>7.2182624999999989</v>
       </c>
-      <c r="T3">
+      <c r="T3" s="3">
         <f>(0.083 + 0.073) *$Q3 - (0.073 *$C3)</f>
         <v>39.037462500000004</v>
       </c>
-      <c r="U3">
+      <c r="U3" s="3">
         <f>0.015 * 2 *$Q3 - (0.015 *$C3)</f>
         <v>6.9302812499999984</v>
       </c>
@@ -639,19 +639,19 @@
         <f t="shared" si="2"/>
         <v>913.79812499999991</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="3">
         <f>0.093 *$C4</f>
         <v>83.7</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="3">
         <f>(0.01275 + (0.0025*(G4=FALSE)*(E4&gt;=23))) *C4</f>
         <v>13.725</v>
       </c>
-      <c r="T4">
+      <c r="T4" s="3">
         <f>0.083 *$C4</f>
         <v>74.7</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="3">
         <f>0.015 *$C4</f>
         <v>13.5</v>
       </c>
@@ -699,19 +699,19 @@
         <f t="shared" si="2"/>
         <v>1296.586875</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="3">
         <f>0.093 *$C5</f>
         <v>111.6</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="3">
         <f>(0.01275 + (0.0025*(G5=FALSE)*(E5&gt;=23))) *C5</f>
         <v>15.299999999999999</v>
       </c>
-      <c r="T5">
+      <c r="T5" s="3">
         <f>0.083 *$C5</f>
         <v>99.600000000000009</v>
       </c>
-      <c r="U5">
+      <c r="U5" s="3">
         <f>0.015 *$C5</f>
         <v>18</v>
       </c>
@@ -759,19 +759,19 @@
         <f t="shared" si="2"/>
         <v>1679.3756249999999</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="3">
         <f>0.093 *$C6</f>
         <v>139.5</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="3">
         <f>(0.01275 + (0.0025*(G6=FALSE)*(E6&gt;=23))) *C6</f>
         <v>19.125</v>
       </c>
-      <c r="T6">
+      <c r="T6" s="3">
         <f>0.083 *$C6</f>
         <v>124.5</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="3">
         <f>0.015 *$C6</f>
         <v>22.5</v>
       </c>
@@ -819,19 +819,19 @@
         <f t="shared" si="2"/>
         <v>6145.2443749999993</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="3">
         <f>0.093 *$C7</f>
         <v>465</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="3">
         <f>(0.01275 + (0.0025*(G7=FALSE)*(E7&gt;=23))) *4425</f>
         <v>56.418749999999996</v>
       </c>
-      <c r="T7">
+      <c r="T7" s="3">
         <f>0.083 *4425</f>
         <v>367.27500000000003</v>
       </c>
-      <c r="U7">
+      <c r="U7" s="3">
         <f>0.015 *$C7</f>
         <v>75</v>
       </c>
@@ -879,16 +879,16 @@
         <f>0.7585*450+(((800/(800-450))-(450/(800-450)*0.7585))*(C8-450))</f>
         <v>144.75000000000003</v>
       </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8">
+      <c r="R8" s="3">
+        <v>0</v>
+      </c>
+      <c r="S8" s="3">
+        <v>0</v>
+      </c>
+      <c r="T8" s="3">
+        <v>0</v>
+      </c>
+      <c r="U8" s="3">
         <v>0</v>
       </c>
     </row>
@@ -935,19 +935,19 @@
         <f>0.7585*400+(((800/(800-400))-(400/(800-400)*0.7585))*(C9-400))</f>
         <v>551.70000000000005</v>
       </c>
-      <c r="R9">
+      <c r="R9" s="3">
         <f>0.0995 * 2 *$Q9 - (0.0995 *$C9)</f>
         <v>50.088300000000018</v>
       </c>
-      <c r="S9">
+      <c r="S9" s="3">
         <f>0.00975*2*$Q9-(0.00975*$C9)+(0.0025*(G9=FALSE)*(E9&gt;=23)*Q9)</f>
         <v>4.9081500000000009</v>
       </c>
-      <c r="T9">
+      <c r="T9" s="3">
         <f>(0.079 + 0.07) *$Q9 - (0.07 *$C9)</f>
         <v>40.203300000000006</v>
       </c>
-      <c r="U9">
+      <c r="U9" s="3">
         <f>0.014 * 2 *$Q9 - (0.014 *$C9)</f>
         <v>7.047600000000001</v>
       </c>
@@ -995,19 +995,19 @@
         <f>0.7585*400+(((800/(800-400))-(400/(800-400)*0.7585))*(C10-400))</f>
         <v>924.15</v>
       </c>
-      <c r="R10">
+      <c r="R10" s="3">
         <f>0.0995 *$C10</f>
         <v>89.550000000000011</v>
       </c>
-      <c r="S10">
+      <c r="S10" s="3">
         <f>(0.00975 + (0.0025*(G10=FALSE)*(E10&gt;=23))) *C10</f>
         <v>8.7750000000000004</v>
       </c>
-      <c r="T10">
+      <c r="T10" s="3">
         <f>0.079 *$C10</f>
         <v>71.099999999999994</v>
       </c>
-      <c r="U10">
+      <c r="U10" s="3">
         <f>0.014 *$C10</f>
         <v>12.6</v>
       </c>
@@ -1055,19 +1055,19 @@
         <f>0.7585*400+(((800/(800-400))-(400/(800-400)*0.7585))*(C11-400))</f>
         <v>1296.5999999999999</v>
       </c>
-      <c r="R11">
+      <c r="R11" s="3">
         <f>0.0995 *$C11</f>
         <v>119.4</v>
       </c>
-      <c r="S11">
+      <c r="S11" s="3">
         <f>(0.00975 + (0.0025*(G11=TRUE)*(E11&gt;=23))) *C11</f>
         <v>11.7</v>
       </c>
-      <c r="T11">
+      <c r="T11" s="3">
         <f>0.079 *$C11</f>
         <v>94.8</v>
       </c>
-      <c r="U11">
+      <c r="U11" s="3">
         <f>0.014 *$C11</f>
         <v>16.8</v>
       </c>
@@ -1115,19 +1115,19 @@
         <f>0.7585*400+(((800/(800-400))-(400/(800-400)*0.7585))*(C12-400))</f>
         <v>1669.0500000000002</v>
       </c>
-      <c r="R12">
+      <c r="R12" s="3">
         <f>0.0995 *$C12</f>
         <v>149.25</v>
       </c>
-      <c r="S12">
+      <c r="S12" s="3">
         <f>(0.00975 + (0.0025*(G12=TRUE)*(E12&gt;=23))) *C12</f>
         <v>14.625</v>
       </c>
-      <c r="T12">
+      <c r="T12" s="3">
         <f>0.079 *$C12</f>
         <v>118.5</v>
       </c>
-      <c r="U12">
+      <c r="U12" s="3">
         <f>0.014 *$C12</f>
         <v>21</v>
       </c>
@@ -1175,19 +1175,19 @@
         <f>0.7585*400+(((800/(800-400))-(400/(800-400)*0.7585))*(C13-400))</f>
         <v>9738.7999999999993</v>
       </c>
-      <c r="R13">
+      <c r="R13" s="3">
         <f>0.0995 *5500</f>
         <v>547.25</v>
       </c>
-      <c r="S13">
+      <c r="S13" s="3">
         <f>(0.00975 + (0.0025*(G13=TRUE)*(E13&gt;=23))) *3750</f>
         <v>36.5625</v>
       </c>
-      <c r="T13">
+      <c r="T13" s="3">
         <f>0.079 *3750</f>
         <v>296.25</v>
       </c>
-      <c r="U13">
+      <c r="U13" s="3">
         <f>0.014 *5500</f>
         <v>77</v>
       </c>

</xml_diff>